<commit_message>
Ajout du dossier IXISPI
</commit_message>
<xml_diff>
--- a/7_Suspension/Fichiers_Suspension/Liste_A3.xlsx
+++ b/7_Suspension/Fichiers_Suspension/Liste_A3.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="19">
   <si>
     <t>Nom Code Plaque</t>
   </si>
@@ -46,10 +46,34 @@
     <t>Statut code IMB</t>
   </si>
   <si>
-    <t>CEMRN2SP_1022</t>
+    <t>CEMRJ1CO_1013</t>
   </si>
   <si>
     <t>Liste A3</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/01RA</t>
+  </si>
+  <si>
+    <t>Qualif Négo</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/01UB</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/01UC</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/01UD</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/02HU</t>
+  </si>
+  <si>
+    <t>IMB/26198/C/02MG</t>
   </si>
 </sst>
 </file>
@@ -113,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -121,6 +145,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +440,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,6 +486,132 @@
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="3"/>
+    </row>
   </sheetData>
   <autoFilter ref="A3:G3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>